<commit_message>
tipo en seleccionador de partidos y partidos seleccionados para comenzar la proxima
</commit_message>
<xml_diff>
--- a/fixture_pre_armado.xlsx
+++ b/fixture_pre_armado.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Documents\TP FINAL MMAD\Fixture-Playoffs-America-Cup\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DB5235-1DE0-42D3-B3ED-AAC909A1CE3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Fixture" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="21">
   <si>
     <t>Team</t>
   </si>
@@ -53,13 +47,43 @@
   </si>
   <si>
     <t>VEN</t>
+  </si>
+  <si>
+    <t>@PER</t>
+  </si>
+  <si>
+    <t>@COL</t>
+  </si>
+  <si>
+    <t>@ECU</t>
+  </si>
+  <si>
+    <t>@CHI</t>
+  </si>
+  <si>
+    <t>@ARG</t>
+  </si>
+  <si>
+    <t>@PAR</t>
+  </si>
+  <si>
+    <t>@BOL</t>
+  </si>
+  <si>
+    <t>@BRA</t>
+  </si>
+  <si>
+    <t>@VEN</t>
+  </si>
+  <si>
+    <t>@URU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,14 +93,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -104,29 +120,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -168,7 +175,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -200,27 +207,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -252,24 +241,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -445,16 +416,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:S12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,258 +482,237 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+      <c r="R2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O6" t="s">
+        <v>3</v>
+      </c>
+      <c r="R6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" t="s">
+        <v>9</v>
+      </c>
+      <c r="N8" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>20</v>
+      </c>
+      <c r="R8" t="s">
+        <v>12</v>
+      </c>
+      <c r="S8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9" t="s">
+        <v>5</v>
+      </c>
+      <c r="N9" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" t="s">
+        <v>6</v>
+      </c>
+      <c r="M10" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>5</v>
+      </c>
+      <c r="R11" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix de restricciones esquema_miniumax
</commit_message>
<xml_diff>
--- a/fixture_pre_armado.xlsx
+++ b/fixture_pre_armado.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
   <si>
     <t>Team</t>
   </si>
@@ -49,13 +49,25 @@
     <t>VEN</t>
   </si>
   <si>
+    <t>@ECU</t>
+  </si>
+  <si>
+    <t>@URU</t>
+  </si>
+  <si>
     <t>@PER</t>
   </si>
   <si>
     <t>@COL</t>
   </si>
   <si>
-    <t>@ECU</t>
+    <t>@VEN</t>
+  </si>
+  <si>
+    <t>@BRA</t>
+  </si>
+  <si>
+    <t>@PAR</t>
   </si>
   <si>
     <t>@CHI</t>
@@ -64,19 +76,7 @@
     <t>@ARG</t>
   </si>
   <si>
-    <t>@PAR</t>
-  </si>
-  <si>
     <t>@BOL</t>
-  </si>
-  <si>
-    <t>@BRA</t>
-  </si>
-  <si>
-    <t>@VEN</t>
-  </si>
-  <si>
-    <t>@URU</t>
   </si>
 </sst>
 </file>
@@ -486,46 +486,28 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
+      <c r="K2" t="s">
+        <v>4</v>
       </c>
       <c r="M2" t="s">
-        <v>13</v>
-      </c>
-      <c r="R2" t="s">
-        <v>10</v>
-      </c>
-      <c r="S2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" t="s">
-        <v>7</v>
-      </c>
-      <c r="N3" t="s">
-        <v>11</v>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -535,31 +517,31 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" t="s">
-        <v>17</v>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" t="s">
+        <v>10</v>
       </c>
       <c r="O4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>8</v>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" t="s">
+        <v>19</v>
+      </c>
+      <c r="P5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -567,28 +549,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
       </c>
-      <c r="J6" t="s">
-        <v>19</v>
-      </c>
       <c r="M6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O6" t="s">
         <v>3</v>
-      </c>
-      <c r="R6" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -599,22 +569,16 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
       </c>
-      <c r="F7" t="s">
-        <v>4</v>
-      </c>
       <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L7" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="M7" t="s">
         <v>1</v>
@@ -625,57 +589,27 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G8" t="s">
         <v>6</v>
-      </c>
-      <c r="L8" t="s">
-        <v>17</v>
-      </c>
-      <c r="M8" t="s">
-        <v>9</v>
-      </c>
-      <c r="N8" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>20</v>
-      </c>
-      <c r="R8" t="s">
-        <v>12</v>
-      </c>
-      <c r="S8" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
       <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" t="s">
         <v>12</v>
       </c>
       <c r="M9" t="s">
         <v>5</v>
       </c>
-      <c r="N9" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>14</v>
+      <c r="R9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -683,33 +617,39 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" t="s">
+        <v>8</v>
       </c>
       <c r="L10" t="s">
         <v>6</v>
       </c>
-      <c r="M10" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>7</v>
+      <c r="P10" t="s">
+        <v>2</v>
+      </c>
+      <c r="R10" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" t="s">
-        <v>1</v>
-      </c>
-      <c r="J11" t="s">
-        <v>5</v>
-      </c>
-      <c r="R11" t="s">
-        <v>15</v>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="M11" t="s">
+        <v>16</v>
+      </c>
+      <c r="P11" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>